<commit_message>
source data for figure 1
</commit_message>
<xml_diff>
--- a/figure1.xlsx
+++ b/figure1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/TakumaWatari/Dropbox/GitHub/concrete-flows-global/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E6D7887-A597-F341-A905-D3AF22DA272A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE245E14-C1CE-4241-8787-87CAA9D3D848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="860" yWindow="-19060" windowWidth="27500" windowHeight="16440" xr2:uid="{81B25FAE-D7FB-474E-864A-C5B27A48FFA5}"/>
   </bookViews>
@@ -738,7 +738,7 @@
         <v>21</v>
       </c>
       <c r="D13" s="2">
-        <v>6.757501252918015</v>
+        <v>8.8594435529009523</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -752,7 +752,7 @@
         <v>22</v>
       </c>
       <c r="D14" s="2">
-        <v>8.7176924560545377</v>
+        <v>6.8673793220711534</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -794,7 +794,7 @@
         <v>22</v>
       </c>
       <c r="D17" s="2">
-        <v>3.846402113113021</v>
+        <v>3.9089452369034769</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1032,7 +1032,7 @@
         <v>32</v>
       </c>
       <c r="D34" s="2">
-        <v>203.60647134152347</v>
+        <v>13.90659595256632</v>
       </c>
       <c r="E34" t="s">
         <v>40</v>
@@ -1049,7 +1049,7 @@
         <v>33</v>
       </c>
       <c r="D35" s="2">
-        <v>205.19697142782482</v>
+        <v>14.015229248536631</v>
       </c>
       <c r="E35" t="s">
         <v>40</v>
@@ -1066,7 +1066,7 @@
         <v>34</v>
       </c>
       <c r="D36" s="2">
-        <v>182.6556408353693</v>
+        <v>12.47562603888869</v>
       </c>
       <c r="E36" t="s">
         <v>40</v>

</xml_diff>